<commit_message>
[Hien Nguyen] Update status for bug 47
</commit_message>
<xml_diff>
--- a/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
+++ b/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
@@ -1110,7 +1110,49 @@
              Thieu tai khoan PL cua VAT </t>
   </si>
   <si>
-    <t>[02-Oct Hien] 
+    <t>[30-Sep Hien] 
+- Disable currency in tab MT910, get value of Currency from tab Main
+- Hide "Nostro Account" on UI, need to check impact on DB
+- Remove "Ordering Institution Address 1/2/3" and "intermediary Address 1/2/3" labels</t>
+  </si>
+  <si>
+    <t>[30-Sep Hien]
+- Changed "Transfer Slip" to "Phieu Chuyen Khoan"</t>
+  </si>
+  <si>
+    <t>[02-Oct Hien]
+- Report file is exported
+- Gettting data from DB to fill in export file (Ongoing)
+[30-Sep Hien]
+- Add function to report Phieu Xuat Ngoai Bang
+- Check for template of Phieu Xuat Ngoai Bang with a.Nguyen</t>
+  </si>
+  <si>
+    <t>[02-Oct Hien]
+Done
+[28-July-2015][BIS] Raised Bug62 to check. Anh Nguyen check lai dum, day co phai la new Requirement?</t>
+  </si>
+  <si>
+    <t>[03-Oct Hien]
+- Removed filed
+- Confirm with aNguyen for formual which is used to calculate drFromAmmount</t>
+  </si>
+  <si>
+    <t>[03-Oct Hien]
+Done
+[1-10 Hien]
+- Removed filed</t>
+  </si>
+  <si>
+    <t>[03-10 Hien]
+- added number as required 
+- confirm a.Nguyen for number at "Address" fill or not fill number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[04-Oct Hien]
+- confirmed wih aNguyen, don't need PL for VAT.
+- Added space between "USD" and value
+[02-Oct Hien] 
 - Confirm with aNguyen for value of PL account at total VAT. There're many PL accounts, which PL should be shown.
 [30-Sep Hien]
 - Hide Oversea Mnus &amp; Plus
@@ -1119,52 +1161,14 @@
 2.Display value of amount (Tab 910) = Drawing Amount (Main) -BB + BC
 --&gt; lam sau
 Lưu ý: Phiếu báo có, Nợ tk Nostro tabMain/field 19, Có hoặc tk KH tabMain (Drawer) hoặc tk Thu Chi Hộ
-Check voi aNguyen vao T2</t>
-  </si>
-  <si>
-    <t>[30-Sep Hien] 
-- Disable currency in tab MT910, get value of Currency from tab Main
-- Hide "Nostro Account" on UI, need to check impact on DB
-- Remove "Ordering Institution Address 1/2/3" and "intermediary Address 1/2/3" labels</t>
-  </si>
-  <si>
-    <t>[30-Sep Hien]
-- Changed "Transfer Slip" to "Phieu Chuyen Khoan"</t>
-  </si>
-  <si>
-    <t>[02-Oct Hien]
-- Report file is exported
-- Gettting data from DB to fill in export file (Ongoing)
-[30-Sep Hien]
-- Add function to report Phieu Xuat Ngoai Bang
-- Check for template of Phieu Xuat Ngoai Bang with a.Nguyen</t>
-  </si>
-  <si>
-    <t>[02-Oct Hien]
-Done
-[28-July-2015][BIS] Raised Bug62 to check. Anh Nguyen check lai dum, day co phai la new Requirement?</t>
-  </si>
-  <si>
-    <t>[03-Oct Hien]
-- Removed filed
-- Confirm with aNguyen for formual which is used to calculate drFromAmmount</t>
-  </si>
-  <si>
-    <t>[03-Oct Hien]
-Done
-[1-10 Hien]
-- Removed filed</t>
-  </si>
-  <si>
-    <t>[03-10 Hien]
-- added number as required 
-- confirm a.Nguyen for number at "Address" fill or not fill number</t>
+Check voi aNguyen vao T2
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2268,10 +2272,10 @@
   <dimension ref="A2:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L48" sqref="L48"/>
+      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,7 +3676,7 @@
         <v>17</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3692,7 +3696,7 @@
         <v>17</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -3754,7 +3758,7 @@
         <v>16</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3833,7 +3837,7 @@
         <v>17</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="90" x14ac:dyDescent="0.25">
@@ -3856,7 +3860,7 @@
         <v>16</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4198,7 +4202,7 @@
         <v>17</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4276,7 +4280,7 @@
         <v>17</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -4302,7 +4306,7 @@
         <v>17</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Hien Nguyen] commit for new template file
</commit_message>
<xml_diff>
--- a/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
+++ b/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="310">
   <si>
     <t>Category</t>
   </si>
@@ -887,10 +887,6 @@
     <t>[Nghia] anh Nguyen check lai loi nay dum em, hien tai minh cung ko tinh VAT cho BB va BC, voi lai tren testing site, Party Charged van con enable, no nen read only.</t>
   </si>
   <si>
-    <t>[30-July-2015]BIS- Hien tai Accept va Register su dung chung function, chung VAT document template.
-[28-July-2015] [BIS] Raised Bug61 to chek</t>
-  </si>
-  <si>
     <t>- Khong in duoc</t>
   </si>
   <si>
@@ -1121,14 +1117,6 @@
   </si>
   <si>
     <t>[02-Oct Hien]
-- Report file is exported
-- Gettting data from DB to fill in export file (Ongoing)
-[30-Sep Hien]
-- Add function to report Phieu Xuat Ngoai Bang
-- Check for template of Phieu Xuat Ngoai Bang with a.Nguyen</t>
-  </si>
-  <si>
-    <t>[02-Oct Hien]
 Done
 [28-July-2015][BIS] Raised Bug62 to check. Anh Nguyen check lai dum, day co phai la new Requirement?</t>
   </si>
@@ -1149,7 +1137,9 @@
 - confirm a.Nguyen for number at "Address" fill or not fill number</t>
   </si>
   <si>
-    <t xml:space="preserve">[04-Oct Hien]
+    <t xml:space="preserve">[6-10 Hien]
+Done except VAT NO, Store Procudure's working fine but there's not information stored in DB (table BOUTGOINGCOLLECTIONPAYMENTCHARGES, check with aNguyen to get more information)
+[04-Oct Hien]
 - confirmed wih aNguyen, don't need PL for VAT.
 - Added space between "USD" and value
 [02-Oct Hien] 
@@ -1164,11 +1154,36 @@
 Check voi aNguyen vao T2
 </t>
   </si>
+  <si>
+    <t>[6-Oct Hien] Done
+[02-Oct Hien]
+- Report file is exported
+- Gettting data from DB to fill in export file (Ongoing)
+[30-Sep Hien]
+- Add function to report Phieu Xuat Ngoai Bang
+- Check for template of Phieu Xuat Ngoai Bang with a.Nguyen</t>
+  </si>
+  <si>
+    <t>[06-Oct Hien]
+Ongoing, will be done by today
+[30-July-2015]BIS- Hien tai Accept va Register su dung chung function, chung VAT document template.
+[28-July-2015] [BIS] Raised Bug61 to chek</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>[06-Oct Hien]
+Ongoing, will try to finish by tomorrow</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="B1dd\-mmm\-yy"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1328,7 +1343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1384,6 +1399,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2071,9 +2089,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2101,7 +2119,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>197</v>
@@ -2120,7 +2138,7 @@
       </c>
       <c r="C4" s="7">
         <f>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -2136,7 +2154,7 @@
       </c>
       <c r="C5" s="7">
         <f>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>196</v>
@@ -2174,7 +2192,7 @@
       </c>
       <c r="C7" s="7">
         <f>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>198</v>
@@ -2225,7 +2243,7 @@
       </c>
       <c r="C10" s="8">
         <f>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>194</v>
@@ -2272,10 +2290,10 @@
   <dimension ref="A2:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,11 +3690,17 @@
       <c r="E47" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H47" s="21">
+        <v>42280</v>
+      </c>
+      <c r="I47" s="21">
+        <v>42280</v>
+      </c>
       <c r="J47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3690,13 +3714,19 @@
         <v>178</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+      <c r="H48" s="21">
+        <v>42277</v>
+      </c>
+      <c r="I48" s="21">
+        <v>42277</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -3704,26 +3734,26 @@
         <v>23</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3737,7 +3767,7 @@
         <v>182</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>21</v>
@@ -3748,17 +3778,17 @@
       <c r="G52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H52" s="4">
-        <v>42194</v>
-      </c>
-      <c r="I52" s="4">
-        <v>42194</v>
+      <c r="H52" s="21">
+        <v>42277</v>
+      </c>
+      <c r="I52" s="21">
+        <v>42283</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3797,10 +3827,10 @@
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>280</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>21</v>
@@ -3822,7 +3852,7 @@
         <v>187</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>21</v>
@@ -3831,16 +3861,22 @@
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
+      </c>
+      <c r="H55" s="21">
+        <v>42277</v>
+      </c>
+      <c r="I55" s="21">
+        <v>42277</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>189</v>
       </c>
@@ -3851,16 +3887,22 @@
         <v>186</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H56" s="21">
+        <v>42277</v>
+      </c>
+      <c r="I56" s="21">
+        <v>42283</v>
+      </c>
       <c r="J56" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -3885,10 +3927,10 @@
       <c r="G57" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H57" s="4">
+      <c r="H57" s="21">
         <v>42198</v>
       </c>
-      <c r="I57" s="4">
+      <c r="I57" s="21">
         <v>41833</v>
       </c>
       <c r="J57" s="1" t="s">
@@ -3917,10 +3959,10 @@
       <c r="G58" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H58" s="21">
         <v>42201</v>
       </c>
-      <c r="I58" s="4">
+      <c r="I58" s="21">
         <v>42201</v>
       </c>
       <c r="J58" s="1" t="s">
@@ -3949,10 +3991,10 @@
       <c r="G59" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="21">
         <v>42201</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I59" s="21">
         <v>42201</v>
       </c>
       <c r="J59" s="1" t="s">
@@ -3981,10 +4023,10 @@
       <c r="G60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="21">
         <v>42201</v>
       </c>
-      <c r="I60" s="4">
+      <c r="I60" s="21">
         <v>42201</v>
       </c>
       <c r="J60" s="1" t="s">
@@ -4013,10 +4055,10 @@
       <c r="G61" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="21">
         <v>42201</v>
       </c>
-      <c r="I61" s="4">
+      <c r="I61" s="21">
         <v>42201</v>
       </c>
       <c r="J61" s="1" t="s">
@@ -4036,6 +4078,8 @@
       <c r="E62" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
       <c r="J62" s="1" t="s">
         <v>192</v>
       </c>
@@ -4062,10 +4106,10 @@
       <c r="G63" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="21">
         <v>42201</v>
       </c>
-      <c r="I63" s="4">
+      <c r="I63" s="21">
         <v>42201</v>
       </c>
       <c r="J63" s="1" t="s">
@@ -4097,10 +4141,10 @@
       <c r="G64" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H64" s="21">
         <v>42205</v>
       </c>
-      <c r="I64" s="4">
+      <c r="I64" s="21">
         <v>42205</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -4126,6 +4170,8 @@
       <c r="G65" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
       <c r="J65" s="1" t="s">
         <v>150</v>
       </c>
@@ -4152,10 +4198,10 @@
       <c r="G66" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H66" s="4">
+      <c r="H66" s="21">
         <v>42215</v>
       </c>
-      <c r="I66" s="4">
+      <c r="I66" s="21">
         <v>42215</v>
       </c>
       <c r="J66" s="1" t="s">
@@ -4165,7 +4211,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>232</v>
       </c>
@@ -4176,13 +4222,17 @@
         <v>231</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="H67" s="21">
+        <v>42283</v>
+      </c>
+      <c r="I67" s="21"/>
       <c r="J67" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>243</v>
+        <v>307</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -4196,13 +4246,19 @@
         <v>233</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="H68" s="21">
+        <v>42279</v>
+      </c>
+      <c r="I68" s="21">
+        <v>42279</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4224,10 +4280,10 @@
       <c r="G69" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H69" s="4">
+      <c r="H69" s="21">
         <v>42215</v>
       </c>
-      <c r="I69" s="4">
+      <c r="I69" s="21">
         <v>42215</v>
       </c>
       <c r="J69" s="1" t="s">
@@ -4250,8 +4306,10 @@
       <c r="F70" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
       <c r="J70" s="1" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="L70" s="19" t="s">
         <v>242</v>
@@ -4259,16 +4317,16 @@
     </row>
     <row r="71" spans="1:12" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>22</v>
@@ -4276,25 +4334,31 @@
       <c r="F71" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H71" s="21">
+        <v>42280</v>
+      </c>
+      <c r="I71" s="21">
+        <v>42280</v>
+      </c>
       <c r="J71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>22</v>
@@ -4302,25 +4366,31 @@
       <c r="F72" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H72" s="21">
+        <v>42280</v>
+      </c>
+      <c r="I72" s="21">
+        <v>42280</v>
+      </c>
       <c r="J72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>22</v>
@@ -4328,23 +4398,30 @@
       <c r="F73" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
       <c r="J73" s="1" t="s">
-        <v>15</v>
+        <v>308</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>282</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
     </row>
     <row r="75" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -4354,10 +4431,10 @@
         <v>23</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>22</v>
@@ -4365,6 +4442,8 @@
       <c r="F75" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
       <c r="J75" s="1" t="s">
         <v>15</v>
       </c>
@@ -4377,10 +4456,10 @@
         <v>23</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>22</v>
@@ -4388,6 +4467,8 @@
       <c r="F76" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
       <c r="J76" s="1" t="s">
         <v>15</v>
       </c>
@@ -4400,10 +4481,10 @@
         <v>23</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>22</v>
@@ -4411,6 +4492,8 @@
       <c r="F77" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
       <c r="J77" s="1" t="s">
         <v>15</v>
       </c>
@@ -4420,10 +4503,10 @@
         <v>23</v>
       </c>
       <c r="C78" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>21</v>
@@ -4431,6 +4514,8 @@
       <c r="F78" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
       <c r="J78" s="1" t="s">
         <v>15</v>
       </c>
@@ -4438,66 +4523,78 @@
     <row r="79" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B79" s="17"/>
       <c r="C79" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>284</v>
-      </c>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
     </row>
     <row r="80" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B80" s="17"/>
       <c r="C80" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
     </row>
     <row r="81" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="17"/>
       <c r="C81" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>287</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
     </row>
     <row r="82" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="17"/>
       <c r="C82" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>289</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
     </row>
     <row r="83" spans="2:12" ht="135" x14ac:dyDescent="0.25">
       <c r="B83" s="17"/>
       <c r="C83" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
     </row>
     <row r="84" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="17"/>
       <c r="C84" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>292</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
     </row>
     <row r="85" spans="2:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>21</v>
@@ -4506,16 +4603,16 @@
         <v>13</v>
       </c>
       <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
       <c r="J85" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="K85" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="K85" s="14" t="s">
+      <c r="L85" s="23" t="s">
         <v>259</v>
-      </c>
-      <c r="L85" s="22" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="86" spans="2:12" ht="120" x14ac:dyDescent="0.25">
@@ -4523,10 +4620,10 @@
         <v>23</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>21</v>
@@ -4535,25 +4632,25 @@
         <v>12</v>
       </c>
       <c r="G86" s="15"/>
-      <c r="H86" s="15"/>
-      <c r="I86" s="15"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
       <c r="J86" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K86" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="L86" s="23"/>
+        <v>258</v>
+      </c>
+      <c r="L86" s="24"/>
     </row>
     <row r="87" spans="2:12" ht="210" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>21</v>
@@ -4562,10 +4659,10 @@
         <v>12</v>
       </c>
       <c r="G87" s="15"/>
-      <c r="H87" s="15"/>
-      <c r="I87" s="15"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
       <c r="J87" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K87" s="15" t="s">
         <v>21</v>
@@ -4577,10 +4674,10 @@
         <v>23</v>
       </c>
       <c r="C88" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>21</v>
@@ -4588,8 +4685,10 @@
       <c r="F88" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
       <c r="J88" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>21</v>
@@ -4597,10 +4696,10 @@
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>21</v>
@@ -4609,18 +4708,20 @@
         <v>12</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
     </row>
     <row r="90" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>21</v>
@@ -4628,16 +4729,18 @@
       <c r="F90" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
     </row>
     <row r="91" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>21</v>
@@ -4645,13 +4748,15 @@
       <c r="F91" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>21</v>
@@ -4660,15 +4765,17 @@
         <v>12</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
     </row>
     <row r="93" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>21</v>
@@ -4676,16 +4783,18 @@
       <c r="F93" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
       <c r="J93" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C94" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>21</v>
@@ -4693,16 +4802,26 @@
       <c r="F94" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
     </row>
     <row r="95" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C95" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="H95" s="21"/>
+      <c r="I95" s="21"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+    </row>
+    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="1" t="s">
-        <v>294</v>
-      </c>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[Hien Nguyen] Update status
</commit_message>
<xml_diff>
--- a/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
+++ b/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="309">
   <si>
     <t>Category</t>
   </si>
@@ -1170,10 +1170,9 @@
 [28-July-2015] [BIS] Raised Bug61 to chek</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
-    <t>[06-Oct Hien]
+    <t>[09-Oct Hien]
+Done
+[06-Oct Hien]
 Ongoing, will try to finish by tomorrow</t>
   </si>
 </sst>
@@ -2290,10 +2289,10 @@
   <dimension ref="A2:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
+      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4401,10 +4400,10 @@
       <c r="H73" s="21"/>
       <c r="I73" s="21"/>
       <c r="J73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4470,7 +4469,7 @@
       <c r="H76" s="21"/>
       <c r="I76" s="21"/>
       <c r="J76" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -4495,7 +4494,7 @@
       <c r="H77" s="21"/>
       <c r="I77" s="21"/>
       <c r="J77" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -4517,7 +4516,7 @@
       <c r="H78" s="21"/>
       <c r="I78" s="21"/>
       <c r="J78" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -4541,6 +4540,9 @@
       </c>
       <c r="H80" s="21"/>
       <c r="I80" s="21"/>
+      <c r="J80" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="81" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="17"/>
@@ -4552,6 +4554,9 @@
       </c>
       <c r="H81" s="21"/>
       <c r="I81" s="21"/>
+      <c r="J81" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="82" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="17"/>
@@ -4563,6 +4568,9 @@
       </c>
       <c r="H82" s="21"/>
       <c r="I82" s="21"/>
+      <c r="J82" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="83" spans="2:12" ht="135" x14ac:dyDescent="0.25">
       <c r="B83" s="17"/>
@@ -4585,6 +4593,9 @@
       </c>
       <c r="H84" s="21"/>
       <c r="I84" s="21"/>
+      <c r="J84" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="85" spans="2:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">

</xml_diff>

<commit_message>
[Hien Nguyen] Commit change for bug 68 - 78 ((change settlement page like payment page in "Export/Document Collection"
</commit_message>
<xml_diff>
--- a/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
+++ b/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="309">
   <si>
     <t>Category</t>
   </si>
@@ -2289,10 +2289,10 @@
   <dimension ref="A2:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
+      <selection pane="bottomRight" activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,7 +4444,7 @@
       <c r="H75" s="21"/>
       <c r="I75" s="21"/>
       <c r="J75" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -4582,6 +4582,9 @@
       </c>
       <c r="H83" s="21"/>
       <c r="I83" s="21"/>
+      <c r="J83" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="84" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="17"/>

</xml_diff>

<commit_message>
[Hien Nguyen] Update bug status
</commit_message>
<xml_diff>
--- a/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
+++ b/Bugs_tracking/VietVictory_BugTracking_Hien.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="329">
   <si>
     <t>Category</t>
   </si>
@@ -903,12 +903,6 @@
     <t>Export Documentary Processing/Settlement</t>
   </si>
   <si>
-    <t xml:space="preserve">Dựa vào số TF để xác định đó là SP hay MA, sau khi gõ số TF thì trường này tự động lấy giá trị SP/MA tương ứng
-- Neu Adising LC/LC Type la (ELCM,ELCP,ELCS) la SP
-- Neu Adising LC/LC Type la (ELCA,ELCD,ELCU) la MA
-</t>
-  </si>
-  <si>
     <t>Export Documentary Processing/Settlement
 Tab Main/1.1 Draw Type</t>
   </si>
@@ -939,9 +933,6 @@
   <si>
     <t>Lưu ý check lại số tiền bằng chữ ở các phiếu, hóa đơn
 (vd: EUR thì ko có chữ "đồng"…)</t>
-  </si>
-  <si>
-    <t>New arise</t>
   </si>
   <si>
     <t>Tất cả các lỗi này đã email Anh Nguyên trước đây</t>
@@ -1174,6 +1165,72 @@
 Done
 [06-Oct Hien]
 Ongoing, will try to finish by tomorrow</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Bug 69</t>
+  </si>
+  <si>
+    <t>Bug 70</t>
+  </si>
+  <si>
+    <t>Bug 71</t>
+  </si>
+  <si>
+    <t>Bug 72</t>
+  </si>
+  <si>
+    <t>Bug 73</t>
+  </si>
+  <si>
+    <t>Bug 74</t>
+  </si>
+  <si>
+    <t>Bug 75</t>
+  </si>
+  <si>
+    <t>Bug 76</t>
+  </si>
+  <si>
+    <t>Bug 77</t>
+  </si>
+  <si>
+    <t>Bug 78</t>
+  </si>
+  <si>
+    <t>Bug 79</t>
+  </si>
+  <si>
+    <t>Bug 80</t>
+  </si>
+  <si>
+    <t>Bug 81</t>
+  </si>
+  <si>
+    <t>Bug 82</t>
+  </si>
+  <si>
+    <t>Bug 83</t>
+  </si>
+  <si>
+    <t>Bug 84</t>
+  </si>
+  <si>
+    <t>Bug 85</t>
+  </si>
+  <si>
+    <t>Bug 86</t>
+  </si>
+  <si>
+    <t>Bug 87</t>
+  </si>
+  <si>
+    <t>Partial fixed</t>
+  </si>
+  <si>
+    <t>Check with aNguyen data in DataBase</t>
   </si>
 </sst>
 </file>
@@ -1417,48 +1474,46 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="48">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1661,13 +1716,44 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <color rgb="FF006100"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1709,6 +1795,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1727,7 +1864,7 @@
   <autoFilter ref="B2:D11"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Status"/>
-    <tableColumn id="2" name="Counts" dataDxfId="35">
+    <tableColumn id="2" name="Counts" dataDxfId="47">
       <calculatedColumnFormula>COUNTIF(Table1[Status],Table2[[#This Row],[Status]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Remark"/>
@@ -1741,7 +1878,7 @@
   <autoFilter ref="F2:H9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Category"/>
-    <tableColumn id="2" name="Bugs" dataDxfId="34">
+    <tableColumn id="2" name="Bugs" dataDxfId="46">
       <calculatedColumnFormula>COUNTIF(Sheet1!$B:$B,Table3[[#This Row],[Category]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Remarks"/>
@@ -1751,7 +1888,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:L72" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:L72" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A2:L72">
     <filterColumn colId="1">
       <filters>
@@ -1767,18 +1904,18 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="BugNo" dataDxfId="11"/>
-    <tableColumn id="2" name="Category" dataDxfId="10"/>
-    <tableColumn id="3" name="Title" dataDxfId="9"/>
-    <tableColumn id="4" name="Description" dataDxfId="8"/>
-    <tableColumn id="12" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" name="Severiry" dataDxfId="6"/>
-    <tableColumn id="6" name="Asignee" dataDxfId="5"/>
-    <tableColumn id="7" name="Start Date" dataDxfId="4"/>
-    <tableColumn id="8" name="End Date" dataDxfId="3"/>
-    <tableColumn id="11" name="Status" dataDxfId="2"/>
-    <tableColumn id="9" name="Path" dataDxfId="1"/>
-    <tableColumn id="10" name="Remark" dataDxfId="0"/>
+    <tableColumn id="1" name="BugNo" dataDxfId="43"/>
+    <tableColumn id="2" name="Category" dataDxfId="42"/>
+    <tableColumn id="3" name="Title" dataDxfId="41"/>
+    <tableColumn id="4" name="Description" dataDxfId="40"/>
+    <tableColumn id="12" name="Type" dataDxfId="39"/>
+    <tableColumn id="5" name="Severiry" dataDxfId="38"/>
+    <tableColumn id="6" name="Asignee" dataDxfId="37"/>
+    <tableColumn id="7" name="Start Date" dataDxfId="36"/>
+    <tableColumn id="8" name="End Date" dataDxfId="35"/>
+    <tableColumn id="11" name="Status" dataDxfId="34"/>
+    <tableColumn id="9" name="Path" dataDxfId="33"/>
+    <tableColumn id="10" name="Remark" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2262,16 +2399,16 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Not Start"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"On-Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"New"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2289,10 +2426,10 @@
   <dimension ref="A2:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J76" sqref="J76"/>
+      <selection pane="bottomRight" activeCell="K92" sqref="K92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3699,7 +3836,7 @@
         <v>17</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3713,7 +3850,7 @@
         <v>178</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H48" s="21">
         <v>42277</v>
@@ -3725,7 +3862,7 @@
         <v>17</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -3733,26 +3870,26 @@
         <v>23</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3766,7 +3903,7 @@
         <v>182</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>21</v>
@@ -3787,7 +3924,7 @@
         <v>17</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3826,10 +3963,10 @@
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>21</v>
@@ -3851,7 +3988,7 @@
         <v>187</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>21</v>
@@ -3860,7 +3997,7 @@
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H55" s="21">
         <v>42277</v>
@@ -3872,7 +4009,7 @@
         <v>17</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -3901,7 +4038,7 @@
         <v>17</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4231,7 +4368,7 @@
         <v>17</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -4257,7 +4394,7 @@
         <v>17</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4316,16 +4453,16 @@
     </row>
     <row r="71" spans="1:12" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>22</v>
@@ -4343,21 +4480,21 @@
         <v>17</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>22</v>
@@ -4375,18 +4512,18 @@
         <v>17</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>246</v>
@@ -4403,12 +4540,12 @@
         <v>17</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>23</v>
@@ -4417,23 +4554,23 @@
         <v>247</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H74" s="21"/>
       <c r="I74" s="21"/>
     </row>
-    <row r="75" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>248</v>
+        <v>307</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>22</v>
@@ -4449,16 +4586,16 @@
     </row>
     <row r="76" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>21</v>
+        <v>309</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>22</v>
@@ -4474,16 +4611,16 @@
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>22</v>
@@ -4498,14 +4635,17 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="B78" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C78" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>21</v>
@@ -4520,23 +4660,32 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="B79" s="17"/>
       <c r="C79" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H79" s="21"/>
       <c r="I79" s="21"/>
+      <c r="J79" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="80" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="B80" s="17"/>
       <c r="C80" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H80" s="21"/>
       <c r="I80" s="21"/>
@@ -4544,13 +4693,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="17"/>
       <c r="C81" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H81" s="21"/>
       <c r="I81" s="21"/>
@@ -4558,13 +4707,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="B82" s="17"/>
       <c r="C82" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H82" s="21"/>
       <c r="I82" s="21"/>
@@ -4572,13 +4724,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="B83" s="17"/>
       <c r="C83" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H83" s="21"/>
       <c r="I83" s="21"/>
@@ -4586,13 +4741,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="B84" s="17"/>
       <c r="C84" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="H84" s="21"/>
       <c r="I84" s="21"/>
@@ -4600,15 +4758,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="B85" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>21</v>
@@ -4620,24 +4781,27 @@
       <c r="H85" s="21"/>
       <c r="I85" s="21"/>
       <c r="J85" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K85" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="L85" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="K85" s="14" t="s">
+    </row>
+    <row r="86" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="L85" s="23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="86" spans="2:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>21</v>
@@ -4649,22 +4813,25 @@
       <c r="H86" s="21"/>
       <c r="I86" s="21"/>
       <c r="J86" s="15" t="s">
-        <v>260</v>
+        <v>17</v>
       </c>
       <c r="K86" s="15" t="s">
         <v>258</v>
       </c>
       <c r="L86" s="24"/>
     </row>
-    <row r="87" spans="2:12" ht="210" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="B87" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>21</v>
@@ -4676,22 +4843,25 @@
       <c r="H87" s="21"/>
       <c r="I87" s="21"/>
       <c r="J87" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K87" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="L87" s="16"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="K87" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L87" s="16"/>
-    </row>
-    <row r="88" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>21</v>
@@ -4702,18 +4872,21 @@
       <c r="H88" s="21"/>
       <c r="I88" s="21"/>
       <c r="J88" s="1" t="s">
-        <v>263</v>
+        <v>17</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="C89" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>21</v>
@@ -4722,20 +4895,23 @@
         <v>12</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H89" s="21"/>
       <c r="I89" s="21"/>
     </row>
-    <row r="90" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="B90" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>21</v>
@@ -4745,16 +4921,22 @@
       </c>
       <c r="H90" s="21"/>
       <c r="I90" s="21"/>
-    </row>
-    <row r="91" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="J90" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="B91" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>21</v>
@@ -4764,13 +4946,22 @@
       </c>
       <c r="H91" s="21"/>
       <c r="I91" s="21"/>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J91" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="B92" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>21</v>
@@ -4779,17 +4970,20 @@
         <v>12</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H92" s="21"/>
       <c r="I92" s="21"/>
     </row>
-    <row r="93" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>325</v>
+      </c>
       <c r="C93" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>21</v>
@@ -4800,15 +4994,18 @@
       <c r="H93" s="21"/>
       <c r="I93" s="21"/>
       <c r="J93" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="C94" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>21</v>
@@ -4818,21 +5015,24 @@
       </c>
       <c r="H94" s="21"/>
       <c r="I94" s="21"/>
-    </row>
-    <row r="95" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="J94" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C95" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H95" s="21"/>
       <c r="I95" s="21"/>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H96" s="21"/>
       <c r="I96" s="21"/>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D97" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H97" s="21"/>
       <c r="I97" s="21"/>
@@ -4842,72 +5042,100 @@
     <mergeCell ref="L85:L86"/>
   </mergeCells>
   <conditionalFormatting sqref="J60 J62 J64:J68 J1:J58 J70:J1048576">
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"On-hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"Not Reproducible"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J59">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"On-hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Not Reproducible"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J61">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"On-hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Not Reproducible"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J63">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"On-hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Not Reproducible"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"On-hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Not Reproducible"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"On-hold"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"New"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Fixed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Not Reproducible"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"On-hold"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"New"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Fixed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Not Reproducible"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>